<commit_message>
make field names clickable and rearrange fields to match Sean's internal template
</commit_message>
<xml_diff>
--- a/templates/accdcTemplateOutsideSubmission.xlsx
+++ b/templates/accdcTemplateOutsideSubmission.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pende\Documents\01 - PROJECTS\537_observationTemplate\outsideSubmissionTemplate\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pende\Documents\01 - PROJECTS\537_observationTemplate\template\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{583ADAC9-F44B-46DC-94AB-B3E558C67CD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77F2E75-3CC9-4BE3-8CCC-3E1D16BDC9CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9180" yWindow="990" windowWidth="17310" windowHeight="13410" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8385" yWindow="240" windowWidth="20175" windowHeight="15120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="template_v0-00" sheetId="1" r:id="rId1"/>
+    <sheet name="template_v1-00" sheetId="1" r:id="rId1"/>
     <sheet name="README" sheetId="6" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'template_v0-00'!$A$1:$AX$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'template_v1-00'!$A$1:$AZ$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>REFNUM</t>
   </si>
@@ -189,13 +189,22 @@
     <t>OBTIMEend</t>
   </si>
   <si>
-    <t>IMPORTANT</t>
-  </si>
-  <si>
-    <t>Read this doc first: https://github.com/atlanticcanadacdc/outsideSubmissionTemplate/blob/main/docs/accdcHowToSubmitData.pdf</t>
-  </si>
-  <si>
-    <t>To make sure you have to most up-to-date version, download the template directly from our repo: https://github.com/atlanticcanadacdc/outsideSubmissionTemplate</t>
+    <t>Read this doc first:</t>
+  </si>
+  <si>
+    <t>https://github.com/atlanticcanadacdc/outsideSubmissionTemplate/blob/main/docs/accdcHowToSubmitData.pdf</t>
+  </si>
+  <si>
+    <t>To make sure you have to most up-to-date version, download the template directly from our repo:</t>
+  </si>
+  <si>
+    <t>https://github.com/atlanticcanadacdc/template/blob/main/templates/accdcTemplateOutsideSubmission.xlsx</t>
+  </si>
+  <si>
+    <t>OTHERFEATURE</t>
+  </si>
+  <si>
+    <t>SUBNAT</t>
   </si>
 </sst>
 </file>
@@ -206,7 +215,7 @@
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="hh:mm"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -271,8 +280,15 @@
     </font>
     <font>
       <b/>
-      <sz val="16"/>
-      <color theme="1"/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri Light"/>
       <family val="2"/>
       <scheme val="major"/>
@@ -306,7 +322,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -323,19 +339,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -344,12 +351,12 @@
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -666,63 +673,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AX2"/>
+  <dimension ref="A1:AZ2"/>
   <sheetViews>
-    <sheetView topLeftCell="AI1" workbookViewId="0">
-      <selection activeCell="AR12" sqref="AR12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="9.42578125" style="9" customWidth="1"/>
-    <col min="9" max="10" width="9.42578125" style="12" customWidth="1"/>
-    <col min="11" max="11" width="8.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10" style="9" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11" style="9" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="17.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11" style="9" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="17" style="9" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="9" style="9" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="8.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="9" style="9" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="11.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="9.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="38" max="39" width="8.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="9.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="8.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="7.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="9" style="9" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="10.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="14.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="5.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="8.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="10.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="10" style="9" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="9.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="51" max="16384" width="8.85546875" style="9"/>
+    <col min="1" max="1" width="10.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="9.42578125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="8.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" style="9" customWidth="1"/>
+    <col min="11" max="11" width="10.85546875" style="7" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.28515625" style="7" customWidth="1"/>
+    <col min="20" max="20" width="17.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9" style="7" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9" style="7" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="8.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9" style="7" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="11" style="7" customWidth="1"/>
+    <col min="35" max="35" width="8.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="8.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="8.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="9.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="9.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="18.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="11" style="7" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="13.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="10" style="7" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="11" style="7" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="17" style="7" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="14.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="10" style="7" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="9.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="53" max="16384" width="8.85546875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" s="2" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:52" s="2" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -747,134 +758,140 @@
       <c r="H1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="5" t="s">
         <v>49</v>
       </c>
       <c r="K1" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="O1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="M1" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="N1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="R1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="AD1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="AJ1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="AK1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AL1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="AM1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AN1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AO1" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="AP1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AQ1" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="AR1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="AS1" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="AU1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="R1" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="S1" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="T1" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="U1" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="W1" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="X1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y1" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA1" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AV1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AW1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="AE1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="AF1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="AG1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AH1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="AI1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="AJ1" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="AK1" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="AL1" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="AM1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="AN1" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="AO1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="AP1" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="AQ1" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="AR1" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="AS1" s="5" t="s">
+      <c r="AX1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="AT1" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="AU1" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="AV1" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="AW1" s="5" t="s">
+      <c r="AY1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="AX1" s="5" t="s">
+      <c r="AZ1" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:50" s="8" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:52" s="6" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -883,20 +900,20 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
       <c r="K2" s="1"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
       <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
@@ -913,10 +930,10 @@
       <c r="AJ2" s="1"/>
       <c r="AK2" s="1"/>
       <c r="AL2" s="1"/>
-      <c r="AM2" s="1"/>
-      <c r="AN2" s="1"/>
-      <c r="AO2" s="1"/>
-      <c r="AP2" s="1"/>
+      <c r="AM2" s="4"/>
+      <c r="AN2" s="4"/>
+      <c r="AO2" s="4"/>
+      <c r="AP2" s="4"/>
       <c r="AQ2" s="1"/>
       <c r="AR2" s="1"/>
       <c r="AS2" s="1"/>
@@ -925,66 +942,150 @@
       <c r="AV2" s="1"/>
       <c r="AW2" s="1"/>
       <c r="AX2" s="1"/>
+      <c r="AY2" s="1"/>
+      <c r="AZ2" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AX2" xr:uid="{8EF81207-EAEC-4F51-84D0-DB07B3DAFBD3}"/>
-  <dataValidations count="15">
-    <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="yyyy2 must have text length = 4._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" sqref="E1:E1048576" xr:uid="{8759099F-EA84-471E-810A-FFCB466A1148}">
+  <autoFilter ref="A1:AZ2" xr:uid="{8EF81207-EAEC-4F51-84D0-DB07B3DAFBD3}"/>
+  <dataValidations count="24">
+    <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="yyyy2 must have text length = 4._x000a__x000a_See the reference guide at https://github.com/atlanticcanadacdc/template/wiki/Field-metadata#yyyy2" sqref="E1:E1048576" xr:uid="{8759099F-EA84-471E-810A-FFCB466A1148}">
       <formula1>4</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="REFNUM must contain unique values._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" sqref="A1:A1048576" xr:uid="{110F2F1B-99BD-4488-8742-F12721E8BCDB}">
-      <formula1>COUNTIF($A:$A,A1)&lt;2</formula1>
-    </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="dd2 must have a minimum text length of 1 and a maximum text length of 2._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" sqref="G1:G1048576" xr:uid="{D37F2FFA-FF5A-48B4-BB1F-F3255DA4E29C}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="dd2 must have a minimum text length of 1 and a maximum text length of 2._x000a__x000a_See the reference guide at https://github.com/atlanticcanadacdc/template/wiki/Field-metadata#dd2" sqref="G1:G1048576" xr:uid="{D37F2FFA-FF5A-48B4-BB1F-F3255DA4E29C}">
       <formula1>1</formula1>
       <formula2>2</formula2>
     </dataValidation>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" error="LATDEC must have a minimum value of -90 and a maximum value of 90._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" sqref="Q1:Q1048576" xr:uid="{3E3B9040-D53D-4EE4-9942-FD2F4C08E301}">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" error="LATDEC must have a minimum value of -90 and a maximum value of 90._x000a__x000a_See the reference guide at https://github.com/atlanticcanadacdc/template/wiki/Field-metadata#latdec" sqref="AK1:AK1048576" xr:uid="{3E3B9040-D53D-4EE4-9942-FD2F4C08E301}">
       <formula1>-90</formula1>
       <formula2>90</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="LONDEC2 must have a minimum value of -180 and a maximum value of 180._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" sqref="T1:T1048576" xr:uid="{E0963D9F-8EB3-4CAE-9972-F3B4443DD9B2}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="LONDEC2 must have a minimum value of -180 and a maximum value of 180._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" sqref="AN1:AN1048576" xr:uid="{E0963D9F-8EB3-4CAE-9972-F3B4443DD9B2}">
       <formula1>-180</formula1>
       <formula2>180</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="LATDEC2 must have a minimum value of -90 and a maximum value of 90._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" sqref="S1:S1048576" xr:uid="{8EC441BF-CE69-46B2-B117-8DB4DFCF4E67}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="LATDEC2 must have a minimum value of -90 and a maximum value of 90._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" sqref="AM1:AM1048576" xr:uid="{8EC441BF-CE69-46B2-B117-8DB4DFCF4E67}">
       <formula1>-90</formula1>
       <formula2>90</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="LOCUNCM must be a whole number greater than or equal to 10._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" sqref="V1:V1048576" xr:uid="{76877D72-6D7B-4053-9D8A-EF5817DEA169}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="LOCUNCM must be a whole number greater than or equal to 10._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" sqref="AP1:AP1048576" xr:uid="{76877D72-6D7B-4053-9D8A-EF5817DEA169}">
       <formula1>10</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="YYYY must have text length = 4._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" sqref="B1:B1048576" xr:uid="{2B2538EA-15F5-4C6F-9BD7-FFFB59409F9B}">
+    <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="YYYY must have text length = 4._x000a__x000a_See the reference guide at https://github.com/atlanticcanadacdc/template/wiki/Field-metadata#YYYY" sqref="B1:B1048576" xr:uid="{2B2538EA-15F5-4C6F-9BD7-FFFB59409F9B}">
       <formula1>4</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="ELEVmin must be a whole number greater than or equal to 0._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" sqref="AC1:AC1048576" xr:uid="{9DF3AC12-B532-4B95-9071-2B1B0EC4A8B0}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="ELEVmin must be a whole number greater than or equal to 0._x000a__x000a_See the reference guide at https://github.com/atlanticcanadacdc/template/wiki/Field-metadata#elevmin" sqref="AV1:AV1048576" xr:uid="{9DF3AC12-B532-4B95-9071-2B1B0EC4A8B0}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Lowercase text only._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" sqref="AK1:AL1048576" xr:uid="{A03A87E5-1A90-4590-9340-BE069CE30FCB}">
-      <formula1>EXACT(LOWER(AK1),AK1)</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="COLLDUP must be a whole number greater than 0._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" sqref="AU1:AU1048576" xr:uid="{C625A903-796B-43AF-B42E-C1CBF9B064D4}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="COLLDUP must be a whole number greater than 0._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" sqref="AK1:AK1048576 AM1:AN1048576 AP1:AP1048576" xr:uid="{C625A903-796B-43AF-B42E-C1CBF9B064D4}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="MM must have a minimum text length of 1 and a maximum text length of 2._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" sqref="C1:C1048576" xr:uid="{63AA1352-24B0-40CA-9C2F-ED3E31036D5C}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="MM must have a minimum text length of 1 and a maximum text length of 2._x000a__x000a_See the reference guide at https://github.com/atlanticcanadacdc/template/wiki/Field-metadata#mm" sqref="C1:C1048576" xr:uid="{63AA1352-24B0-40CA-9C2F-ED3E31036D5C}">
       <formula1>1</formula1>
       <formula2>2</formula2>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="DD must have a minimum text length of 1 and a maximum text length of 2._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" sqref="D1:D1048576" xr:uid="{60512924-9933-4690-BEF6-28C7301C3ABD}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="DD must have a minimum text length of 1 and a maximum text length of 2._x000a__x000a_See the reference guide at https://github.com/atlanticcanadacdc/template/wiki/Field-metadata#dd" sqref="D1:D1048576" xr:uid="{60512924-9933-4690-BEF6-28C7301C3ABD}">
       <formula1>1</formula1>
       <formula2>2</formula2>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="mm2 must have a minimum text length of 1 and a maximum text length of 2._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" sqref="F1:F1048576" xr:uid="{73F28CD7-CD72-4C1B-8361-F8CBD884DC59}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="mm2 must have a minimum text length of 1 and a maximum text length of 2._x000a__x000a_See the reference guide at https://github.com/atlanticcanadacdc/template/wiki/Field-metadata#mm2" sqref="F1:F1048576" xr:uid="{73F28CD7-CD72-4C1B-8361-F8CBD884DC59}">
       <formula1>1</formula1>
       <formula2>2</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="LONDEC must have a minimum value of -180 and a maximum value of 180._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" sqref="R1:R1048576" xr:uid="{FBE1E6CF-FE6A-454F-8063-F9B3175370DC}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="LONDEC must have a minimum value of -180 and a maximum value of 180._x000a__x000a_See the reference guide at https://github.com/atlanticcanadacdc/template/wiki/Field-metadata#londec" sqref="AL1:AL4 AL6:AL1048576 AL5" xr:uid="{FBE1E6CF-FE6A-454F-8063-F9B3175370DC}">
       <formula1>-180</formula1>
       <formula2>180</formula2>
     </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="REFNUM must contain unique values._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" sqref="B1:G1048576 AJ1:AS1048576" xr:uid="{110F2F1B-99BD-4488-8742-F12721E8BCDB}">
+      <formula1>COUNTIF($A:$A,B1)&lt;2</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Lowercase text only._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" sqref="AJ1:AS1048576 AC1:AF1048576 AC1:AF1048576 AH1:AH1048576 AH1:AH1048576 AJ1:AS1048576" xr:uid="{A03A87E5-1A90-4590-9340-BE069CE30FCB}">
+      <formula1>EXACT(LOWER(AC1),AC1)</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="SUBNAT must be a two letter province code._x000a__x000a_See the reference guide at https://github.com/atlanticcanadacdc/template/wiki/Field-metadata#SUBNAT" sqref="K1:K1048576" xr:uid="{FBCDCF78-1F74-4273-9CBD-4C77E8D31F99}">
+      <formula1>2</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="REFNUM must contain unique values._x000a__x000a_See the reference guide at https://github.com/atlanticcanadacdc/template/wiki/Field-metadata#refnum" sqref="A1:A1048576" xr:uid="{A0E9B4E6-244C-4200-8EC2-65CB3F32A17C}">
+      <formula1>COUNTIF($A:$A,A1)&lt;2</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Lowercase text only._x000a__x000a_See the reference guide at https://github.com/atlanticcanadacdc/template/wiki/Field-metadata#OBPHEN" sqref="AA1:AA1048576" xr:uid="{71CB2089-B43C-49B3-8548-B59F7449CE92}">
+      <formula1>EXACT(LOWER(AA1),AA1)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Lowercase text only. _x000a__x000a_See the reference guide at https://github.com/atlanticcanadacdc/template/wiki/Field-metadata#obabun" sqref="V1:V1048576" xr:uid="{AA0303B4-2632-4F83-89D3-3E033BC9F6E7}">
+      <formula1>EXACT(LOWER(V1),V1)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Lowercase text only._x000a__x000a_See the reference guide at https://github.com/atlanticcanadacdc/template/wiki/Field-metadata#OBSEX" sqref="AB1:AB1048576" xr:uid="{41F36F1F-1BA3-44DA-9550-648085ACD067}">
+      <formula1>EXACT(LOWER(AB1),AB1)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Lowercase text only._x000a__x000a_See the reference guide at https://github.com/atlanticcanadacdc/template/wiki/Field-metadata#protocol" sqref="AG1:AG1048576" xr:uid="{74B2D6D9-5D4B-42E6-9D61-9061D584CA61}">
+      <formula1>EXACT(LOWER(AG1),AG1)</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="COLLDUP must be a whole number greater than 0._x000a__x000a_See the reference guide at https://github.com/atlanticcanadacdc/template/wiki/Field-metadata#colldup" sqref="AI1:AI1048576" xr:uid="{159C0397-B9FB-452A-BBE4-2F7C8290FD47}">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="https://github.com/atlanticcanadacdc/template/wiki/Field-metadata#londec" sqref="AL1:AL1048576" xr:uid="{1BF4A797-5443-48AC-9F0E-7F558C049427}">
+      <formula1>-180</formula1>
+      <formula2>180</formula2>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Lowercase text only._x000a__x000a_See the reference guide at https://github.com/atlanticcanadacdc/template/wiki/Field-metadata#obevid" sqref="AW1:AW1048576" xr:uid="{F2FE263A-5EDB-45C5-A693-77A7C766B3E0}">
+      <formula1>EXACT(LOWER(AW1),AW1)</formula1>
+    </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" location="refnum" xr:uid="{CB419A17-942D-4C93-A976-F2442794B878}"/>
+    <hyperlink ref="B1" r:id="rId2" location="YYYY" xr:uid="{4830192B-280F-4831-BE18-C43CDB2DCE84}"/>
+    <hyperlink ref="C1" r:id="rId3" location="mm" xr:uid="{6CECD1DF-C74E-40EC-ABF1-9966F3C10EBE}"/>
+    <hyperlink ref="D1" r:id="rId4" location="dd" xr:uid="{64C4B1E1-CC6F-4C93-A95C-28E6812AC87D}"/>
+    <hyperlink ref="E1" r:id="rId5" location="yyyy2" xr:uid="{1C137199-6DAA-46D4-B359-E60CB481A179}"/>
+    <hyperlink ref="F1" r:id="rId6" location="mm2" xr:uid="{678C0549-FC7C-4520-8EEA-77E63CFA943E}"/>
+    <hyperlink ref="G1" r:id="rId7" location="dd2" xr:uid="{D9B401AB-73C1-4FD5-9757-9B8BB852A683}"/>
+    <hyperlink ref="H1" r:id="rId8" location="obdateverbatim" xr:uid="{226A41D4-6104-4257-97C1-31E5403DF5D3}"/>
+    <hyperlink ref="I1" r:id="rId9" location="OBTIME" xr:uid="{DE6B4A8C-989E-44DA-A77D-EFB23FA15559}"/>
+    <hyperlink ref="J1" r:id="rId10" location="obtimeend" xr:uid="{BFCA50ED-A0E7-4877-B168-34C98CB4A965}"/>
+    <hyperlink ref="K1" r:id="rId11" location="subnat" xr:uid="{99199E04-F51F-4470-96BA-FCB038FDF75C}"/>
+    <hyperlink ref="L1" r:id="rId12" location="surveysite" xr:uid="{E9AA34AF-10A5-41B1-AC10-9EE443A41E7D}"/>
+    <hyperlink ref="M1" r:id="rId13" location="_notelocsurveysite" xr:uid="{4893B326-A262-46A3-BB78-D31016014B94}"/>
+    <hyperlink ref="N1" r:id="rId14" location="scname" xr:uid="{0A964B0A-5327-4E29-9B5D-921DEE34BB36}"/>
+    <hyperlink ref="O1" r:id="rId15" location="nametemp" xr:uid="{4CB1FAE1-9168-4551-9644-D895681F4E7E}"/>
+    <hyperlink ref="P1" r:id="rId16" location="common-name" xr:uid="{ACD93D75-78FC-48A8-ACB6-9E2B5A81C6D2}"/>
+    <hyperlink ref="Q1" r:id="rId17" location="NOTETAX" xr:uid="{66166F40-3E90-4A8C-9EAF-E1AF1999D3A4}"/>
+    <hyperlink ref="R1" r:id="rId18" location="OBABUNSITE" xr:uid="{F1DFFA4A-61F5-4FDB-85AE-AB5CE6FA6B10}"/>
+    <hyperlink ref="S1" r:id="rId19" location="other-features" xr:uid="{73458A62-27AA-46F3-90A9-4EDBB88EBFC6}"/>
+    <hyperlink ref="T1" r:id="rId20" location="sitecode" xr:uid="{E0CD125B-0A89-443A-BD35-AD74A6333125}"/>
+    <hyperlink ref="U1" r:id="rId21" location="habitat" xr:uid="{05C630F2-A9ED-42E0-A434-6BF1321BC826}"/>
+    <hyperlink ref="V1" r:id="rId22" location="obabun" xr:uid="{2139A2B5-3220-46BD-97C5-B83D8C0E7C92}"/>
+    <hyperlink ref="W1" r:id="rId23" location="OBCOUNT" xr:uid="{B69DF8C8-BEC8-466A-AA3B-55A0E934DE02}"/>
+    <hyperlink ref="X1" r:id="rId24" location="OBASSP" xr:uid="{A04EBB70-F232-40A5-83D6-5D3B78076BBA}"/>
+    <hyperlink ref="Y1" r:id="rId25" location="OBDESC" xr:uid="{96D4B575-CD2F-4E94-AAB0-6B8D1731FDB2}"/>
+    <hyperlink ref="Z1" r:id="rId26" location="OBACTIV" xr:uid="{A6B259A3-4915-4E2C-82D2-7C6267135433}"/>
+    <hyperlink ref="AA1" r:id="rId27" location="OBPHEN" xr:uid="{1E3886FD-7A4E-4069-8524-20185CC4EE4B}"/>
+    <hyperlink ref="AB1" r:id="rId28" location="OBSEX" xr:uid="{3F2F7951-51CA-4FE8-ACBA-5A61D84FCC72}"/>
+    <hyperlink ref="AC1" r:id="rId29" location="OBTHREAT" xr:uid="{30BCC02C-0435-48BC-92EE-B96AEE3BFF59}"/>
+    <hyperlink ref="AD1" r:id="rId30" location="ENVIRONMENTAL" xr:uid="{574C6489-D33C-4BA6-8B11-E8976D8A4727}"/>
+    <hyperlink ref="AE1" r:id="rId31" location="URL" xr:uid="{B6D7C438-F272-482C-B906-0247B0FADDF2}"/>
+    <hyperlink ref="AF1" r:id="rId32" location="project" xr:uid="{6D0DA3B3-5EB3-4240-83F8-FA2DBE01CB80}"/>
+    <hyperlink ref="AG1" r:id="rId33" location="protocol" xr:uid="{1E1D0225-6C8E-43E3-8362-ED370CE424D7}"/>
+    <hyperlink ref="AH1" r:id="rId34" location="collnum" xr:uid="{3280EED9-7E5B-41A2-98EB-29942D5FA879}"/>
+    <hyperlink ref="AI1" r:id="rId35" location="colldup" xr:uid="{EBB423FD-BD65-40CE-8CDE-15BA6296BF80}"/>
+    <hyperlink ref="AJ1" r:id="rId36" location="accnum" xr:uid="{B8DDDB26-27C2-4228-8DBE-B60D5DDF7BEC}"/>
+    <hyperlink ref="AK1" r:id="rId37" location="latdec" xr:uid="{1719AB5A-7EE7-4FA0-A6B3-19AE41899944}"/>
+    <hyperlink ref="AL1" r:id="rId38" location="londec" xr:uid="{834604C0-3879-4AEC-839D-0D78D648EFE3}"/>
+    <hyperlink ref="AM1" r:id="rId39" location="latdec2" xr:uid="{83A98BFE-0D53-4943-B7E7-7EF5974C4393}"/>
+    <hyperlink ref="AN1" r:id="rId40" location="londec2" xr:uid="{6DB04923-8DE7-4FBD-8A3E-09C02373886A}"/>
+    <hyperlink ref="AO1" r:id="rId41" location="_noteloccoordinates" xr:uid="{98930FB5-28CC-413F-968A-885CA7866F07}"/>
+    <hyperlink ref="AP1" r:id="rId42" location="locuncm" xr:uid="{1525876A-AA09-4E00-9BB8-2442C3E6DB49}"/>
+    <hyperlink ref="AQ1" r:id="rId43" location="_NOTELOClocuncm" xr:uid="{AE3F122D-6433-4CEC-8DE5-E082F33E3E36}"/>
+    <hyperlink ref="AR1" r:id="rId44" location="directions" xr:uid="{A1E53390-1C36-4056-BF37-8BD1B5646CBB}"/>
+    <hyperlink ref="AS1" r:id="rId45" location="_notelocdirections" xr:uid="{67F60461-6A06-4471-AB42-D67B35341E44}"/>
+    <hyperlink ref="AT1" r:id="rId46" location="observer" xr:uid="{F88601D1-DCE8-4E18-A1D1-88E16D02FFDB}"/>
+    <hyperlink ref="AU1" r:id="rId47" location="identby" xr:uid="{D3DE2271-2DE8-448D-B2C1-28E55255E885}"/>
+    <hyperlink ref="AV1" r:id="rId48" location="elevmin" xr:uid="{8F13C8E8-B3AA-425C-AF41-E52081E81C65}"/>
+    <hyperlink ref="AW1" r:id="rId49" location="obevid" xr:uid="{3571114C-8AC4-44B0-ADC7-F28FE53ECA68}"/>
+    <hyperlink ref="AX1" r:id="rId50" location="collection" xr:uid="{93D60417-BCDE-4324-B0FD-34842EC37569}"/>
+    <hyperlink ref="AY1" r:id="rId51" location="note1" xr:uid="{AF0D8176-10CC-4474-8491-EE0D335AAFC0}"/>
+    <hyperlink ref="AZ1" r:id="rId52" location="note2" xr:uid="{4668AA28-2B31-4422-8FAF-A3AFFC4FC986}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId53"/>
 </worksheet>
 </file>
 
@@ -992,42 +1093,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B0B503C-45C2-4682-A279-7D9876A20A9B}">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="12" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="13" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
+      <c r="A4" s="12" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
+      <c r="A6" s="10"/>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
+      <c r="A7" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" display="to make sure you have to most up to date version, download this file from our repo: https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" xr:uid="{6915430C-55DD-436F-A74B-E2345D056ECD}"/>
-    <hyperlink ref="A2" r:id="rId2" display="Read this doc first" xr:uid="{6A905369-B841-4FFA-AD4F-39C517722E0D}"/>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{6915430C-55DD-436F-A74B-E2345D056ECD}"/>
+    <hyperlink ref="A1" r:id="rId2" display="Read this doc first" xr:uid="{6A905369-B841-4FFA-AD4F-39C517722E0D}"/>
+    <hyperlink ref="A2" r:id="rId3" xr:uid="{218934DD-FC9D-4F1E-B501-F98FE81D3E67}"/>
+    <hyperlink ref="A4" r:id="rId4" xr:uid="{DF64407A-3DA9-4C8A-9255-459CE474D232}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add link to README tab in outside submission template that redirects to template tab
</commit_message>
<xml_diff>
--- a/templates/accdcTemplateOutsideSubmission.xlsx
+++ b/templates/accdcTemplateOutsideSubmission.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pende\Documents\01 - PROJECTS\537_observationTemplate\template\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pende\Documents\02.1 - WORK AREAS\AC CDC Data Load\template\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77F2E75-3CC9-4BE3-8CCC-3E1D16BDC9CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BAE840-228A-4E4F-9BA2-69F4D168A318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8385" yWindow="240" windowWidth="20175" windowHeight="15120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14505" yWindow="240" windowWidth="14055" windowHeight="15120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="template_v1-00" sheetId="1" r:id="rId1"/>
+    <sheet name="template_v1-01" sheetId="1" r:id="rId1"/>
     <sheet name="README" sheetId="6" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'template_v1-00'!$A$1:$AZ$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'template_v1-01'!$A$1:$AZ$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>REFNUM</t>
   </si>
@@ -205,6 +205,12 @@
   </si>
   <si>
     <t>SUBNAT</t>
+  </si>
+  <si>
+    <t>Enter your data in the first tab of this spreadsheet:</t>
+  </si>
+  <si>
+    <t>template_v1-01</t>
   </si>
 </sst>
 </file>
@@ -675,9 +681,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AZ2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1120,8 +1124,15 @@
         <v>53</v>
       </c>
     </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>56</v>
+      </c>
+    </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
+      <c r="A6" s="12" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
@@ -1132,6 +1143,7 @@
     <hyperlink ref="A1" r:id="rId2" display="Read this doc first" xr:uid="{6A905369-B841-4FFA-AD4F-39C517722E0D}"/>
     <hyperlink ref="A2" r:id="rId3" xr:uid="{218934DD-FC9D-4F1E-B501-F98FE81D3E67}"/>
     <hyperlink ref="A4" r:id="rId4" xr:uid="{DF64407A-3DA9-4C8A-9255-459CE474D232}"/>
+    <hyperlink ref="A6" location="'template_v1-01'!A1" display="template_v1-01" xr:uid="{80375676-F759-4681-9B66-DA4DECEFDFF3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>

</xml_diff>

<commit_message>
update outside submission template README to direct users to the wiki
the how-to document when viewed on GitHub isn't clickable, so assume that if users have this Excel file, they wish to take route 1 and therefore need a direct link to the wiki!
</commit_message>
<xml_diff>
--- a/templates/accdcTemplateOutsideSubmission.xlsx
+++ b/templates/accdcTemplateOutsideSubmission.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pende\Documents\02.1 - WORK AREAS\AC CDC Data Load\template\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BAE840-228A-4E4F-9BA2-69F4D168A318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5291B81-8440-43BC-8B45-1F59D31999BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14505" yWindow="240" windowWidth="14055" windowHeight="15120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2415" yWindow="1620" windowWidth="17175" windowHeight="13215" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template_v1-01" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'template_v1-01'!$A$1:$AZ$2</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -189,15 +189,6 @@
     <t>OBTIMEend</t>
   </si>
   <si>
-    <t>Read this doc first:</t>
-  </si>
-  <si>
-    <t>https://github.com/atlanticcanadacdc/outsideSubmissionTemplate/blob/main/docs/accdcHowToSubmitData.pdf</t>
-  </si>
-  <si>
-    <t>To make sure you have to most up-to-date version, download the template directly from our repo:</t>
-  </si>
-  <si>
     <t>https://github.com/atlanticcanadacdc/template/blob/main/templates/accdcTemplateOutsideSubmission.xlsx</t>
   </si>
   <si>
@@ -211,6 +202,33 @@
   </si>
   <si>
     <t>template_v1-01</t>
+  </si>
+  <si>
+    <t>To make sure you have to most up-to-date version, always download the template directly from our repo:</t>
+  </si>
+  <si>
+    <t>https://github.com/atlanticcanadacdc/template/wiki</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>Remember to click on any field name in the first tab of this spreadsheet</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </rPr>
+      <t xml:space="preserve"> to learn more. You can find the reference guide here:</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -221,7 +239,7 @@
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="hh:mm"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -294,6 +312,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <name val="Calibri Light"/>
       <family val="2"/>
@@ -769,7 +794,7 @@
         <v>49</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>8</v>
@@ -793,7 +818,7 @@
         <v>12</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="T1" s="5" t="s">
         <v>10</v>
@@ -1095,9 +1120,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B0B503C-45C2-4682-A279-7D9876A20A9B}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1106,46 +1133,45 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="13" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>56</v>
+      <c r="A5" s="12" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>57</v>
-      </c>
+      <c r="A6" s="10"/>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
+      <c r="A7" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" xr:uid="{6915430C-55DD-436F-A74B-E2345D056ECD}"/>
-    <hyperlink ref="A1" r:id="rId2" display="Read this doc first" xr:uid="{6A905369-B841-4FFA-AD4F-39C517722E0D}"/>
-    <hyperlink ref="A2" r:id="rId3" xr:uid="{218934DD-FC9D-4F1E-B501-F98FE81D3E67}"/>
-    <hyperlink ref="A4" r:id="rId4" xr:uid="{DF64407A-3DA9-4C8A-9255-459CE474D232}"/>
-    <hyperlink ref="A6" location="'template_v1-01'!A1" display="template_v1-01" xr:uid="{80375676-F759-4681-9B66-DA4DECEFDFF3}"/>
+    <hyperlink ref="A7" r:id="rId1" display="To make sure you have to most up-to-date version, download the template directly from our repo:" xr:uid="{6915430C-55DD-436F-A74B-E2345D056ECD}"/>
+    <hyperlink ref="A8" r:id="rId2" xr:uid="{DF64407A-3DA9-4C8A-9255-459CE474D232}"/>
+    <hyperlink ref="A5" location="'template_v1-01'!A1" display="template_v1-01" xr:uid="{80375676-F759-4681-9B66-DA4DECEFDFF3}"/>
+    <hyperlink ref="A2" r:id="rId3" xr:uid="{7E898EBA-DAC1-4C2D-A2FF-AE781264A37A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update version number to reflect README changes: template_v1-02
</commit_message>
<xml_diff>
--- a/templates/accdcTemplateOutsideSubmission.xlsx
+++ b/templates/accdcTemplateOutsideSubmission.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pende\Documents\02.1 - WORK AREAS\AC CDC Data Load\template\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5291B81-8440-43BC-8B45-1F59D31999BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED28DFCE-335B-4CA2-BBE0-CB1A20724005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2415" yWindow="1620" windowWidth="17175" windowHeight="13215" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9645" yWindow="195" windowWidth="19110" windowHeight="15270" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="template_v1-01" sheetId="1" r:id="rId1"/>
+    <sheet name="template_v1-02" sheetId="1" r:id="rId1"/>
     <sheet name="README" sheetId="6" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'template_v1-01'!$A$1:$AZ$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'template_v1-02'!$A$1:$AZ$2</definedName>
   </definedNames>
   <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
@@ -201,9 +201,6 @@
     <t>Enter your data in the first tab of this spreadsheet:</t>
   </si>
   <si>
-    <t>template_v1-01</t>
-  </si>
-  <si>
     <t>To make sure you have to most up-to-date version, always download the template directly from our repo:</t>
   </si>
   <si>
@@ -229,6 +226,9 @@
       </rPr>
       <t xml:space="preserve"> to learn more. You can find the reference guide here:</t>
     </r>
+  </si>
+  <si>
+    <t>template_v1-02</t>
   </si>
 </sst>
 </file>
@@ -1123,7 +1123,7 @@
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1133,12 +1133,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
@@ -1147,8 +1147,8 @@
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>54</v>
+      <c r="A5" s="10" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
@@ -1156,7 +1156,7 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
@@ -1168,7 +1168,7 @@
   <hyperlinks>
     <hyperlink ref="A7" r:id="rId1" display="To make sure you have to most up-to-date version, download the template directly from our repo:" xr:uid="{6915430C-55DD-436F-A74B-E2345D056ECD}"/>
     <hyperlink ref="A8" r:id="rId2" xr:uid="{DF64407A-3DA9-4C8A-9255-459CE474D232}"/>
-    <hyperlink ref="A5" location="'template_v1-01'!A1" display="template_v1-01" xr:uid="{80375676-F759-4681-9B66-DA4DECEFDFF3}"/>
+    <hyperlink ref="A5" location="'template_v1-02'!A1" display="template_v1-02" xr:uid="{80375676-F759-4681-9B66-DA4DECEFDFF3}"/>
     <hyperlink ref="A2" r:id="rId3" xr:uid="{7E898EBA-DAC1-4C2D-A2FF-AE781264A37A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
select top cell in README on open
</commit_message>
<xml_diff>
--- a/templates/accdcTemplateOutsideSubmission.xlsx
+++ b/templates/accdcTemplateOutsideSubmission.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pende\Documents\02.1 - WORK AREAS\AC CDC Data Load\template\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED28DFCE-335B-4CA2-BBE0-CB1A20724005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{985642AB-B8F3-4C3D-BC32-C256A982B69E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9645" yWindow="195" windowWidth="19110" windowHeight="15270" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1122,9 +1122,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B0B503C-45C2-4682-A279-7D9876A20A9B}">
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
update template with shading of required and recommended fields and add email address to README
</commit_message>
<xml_diff>
--- a/templates/accdcTemplateOutsideSubmission.xlsx
+++ b/templates/accdcTemplateOutsideSubmission.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pende\Documents\02.1 - WORK AREAS\AC CDC Data Load\template\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{985642AB-B8F3-4C3D-BC32-C256A982B69E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{189A1F0A-D370-4D24-9E7F-B1150DCBFD98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9645" yWindow="195" windowWidth="19110" windowHeight="15270" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="template_v1-02" sheetId="1" r:id="rId1"/>
+    <sheet name="template_v1-03" sheetId="1" r:id="rId1"/>
     <sheet name="README" sheetId="6" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'template_v1-02'!$A$1:$AZ$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'template_v1-03'!$A$1:$AZ$2</definedName>
   </definedNames>
-  <calcPr calcId="191029" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>REFNUM</t>
   </si>
@@ -201,10 +201,10 @@
     <t>Enter your data in the first tab of this spreadsheet:</t>
   </si>
   <si>
-    <t>To make sure you have to most up-to-date version, always download the template directly from our repo:</t>
-  </si>
-  <si>
     <t>https://github.com/atlanticcanadacdc/template/wiki</t>
+  </si>
+  <si>
+    <t>template_v1-03</t>
   </si>
   <si>
     <r>
@@ -215,7 +215,7 @@
         <family val="2"/>
         <scheme val="major"/>
       </rPr>
-      <t>Remember to click on any field name in the first tab of this spreadsheet</t>
+      <t>Click on any field name in the first tab of this spreadsheet</t>
     </r>
     <r>
       <rPr>
@@ -224,11 +224,20 @@
         <family val="2"/>
         <scheme val="major"/>
       </rPr>
-      <t xml:space="preserve"> to learn more. You can find the reference guide here:</t>
+      <t xml:space="preserve"> to learn more</t>
     </r>
   </si>
   <si>
-    <t>template_v1-02</t>
+    <t>Spreadsheet reference guide:</t>
+  </si>
+  <si>
+    <t>Always download the template directly from our repo:</t>
+  </si>
+  <si>
+    <t>Once ready, email this spreadsheet to:</t>
+  </si>
+  <si>
+    <t>datasubmissions@accdc.ca</t>
   </si>
 </sst>
 </file>
@@ -353,41 +362,44 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -396,6 +408,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF0563C1"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -710,55 +727,54 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="9.42578125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="7" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.42578125" style="9" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" style="7" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.28515625" style="7" customWidth="1"/>
-    <col min="20" max="20" width="17.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="8.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="10.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="11" style="7" customWidth="1"/>
-    <col min="35" max="35" width="8.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="8.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="8.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="8.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="9.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="9.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="18.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="11" style="7" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="13.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="10" style="7" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="11" style="7" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="17" style="7" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="14.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="10" style="7" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="9.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="9" style="7" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="5.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="10" style="7" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="9.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="8.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="8.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="9.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="9.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="18" style="7" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="10.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="15.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="11" style="7" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="16.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="10" style="7" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="8.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="9" style="7" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="8.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="11.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="51" max="52" width="7.5703125" style="7" bestFit="1" customWidth="1"/>
     <col min="53" max="16384" width="8.85546875" style="7"/>
   </cols>
   <sheetData>
@@ -766,13 +782,13 @@
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="14" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="5" t="s">
@@ -799,10 +815,10 @@
       <c r="L1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="M1" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="14" t="s">
         <v>45</v>
       </c>
       <c r="O1" s="5" t="s">
@@ -871,10 +887,10 @@
       <c r="AJ1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AK1" s="5" t="s">
+      <c r="AK1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="AL1" s="5" t="s">
+      <c r="AL1" s="14" t="s">
         <v>7</v>
       </c>
       <c r="AM1" s="5" t="s">
@@ -883,22 +899,22 @@
       <c r="AN1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="AO1" s="11" t="s">
+      <c r="AO1" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="AP1" s="5" t="s">
+      <c r="AP1" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="AQ1" s="11" t="s">
+      <c r="AQ1" s="13" t="s">
         <v>35</v>
       </c>
       <c r="AR1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="AS1" s="11" t="s">
+      <c r="AS1" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="AT1" s="5" t="s">
+      <c r="AT1" s="14" t="s">
         <v>1</v>
       </c>
       <c r="AU1" s="5" t="s">
@@ -907,7 +923,7 @@
       <c r="AV1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AW1" s="5" t="s">
+      <c r="AW1" s="14" t="s">
         <v>15</v>
       </c>
       <c r="AX1" s="5" t="s">
@@ -976,7 +992,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:AZ2" xr:uid="{8EF81207-EAEC-4F51-84D0-DB07B3DAFBD3}"/>
-  <dataValidations count="24">
+  <dataValidations count="26">
     <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="yyyy2 must have text length = 4._x000a__x000a_See the reference guide at https://github.com/atlanticcanadacdc/template/wiki/Field-metadata#yyyy2" sqref="E1:E1048576" xr:uid="{8759099F-EA84-471E-810A-FFCB466A1148}">
       <formula1>4</formula1>
     </dataValidation>
@@ -984,7 +1000,7 @@
       <formula1>1</formula1>
       <formula2>2</formula2>
     </dataValidation>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" error="LATDEC must have a minimum value of -90 and a maximum value of 90._x000a__x000a_See the reference guide at https://github.com/atlanticcanadacdc/template/wiki/Field-metadata#latdec" sqref="AK1:AK1048576" xr:uid="{3E3B9040-D53D-4EE4-9942-FD2F4C08E301}">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" error="LATDEC must have a minimum value of -90 and a maximum value of 90._x000a__x000a_See the reference guide at https://github.com/atlanticcanadacdc/template/wiki/Field-metadata#latdec" promptTitle="Required field" prompt="Required field. Imprecision in location can be expressed in the LOCUNCM field" sqref="AK1:AK1048576" xr:uid="{3E3B9040-D53D-4EE4-9942-FD2F4C08E301}">
       <formula1>-90</formula1>
       <formula2>90</formula2>
     </dataValidation>
@@ -996,10 +1012,10 @@
       <formula1>-90</formula1>
       <formula2>90</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="LOCUNCM must be a whole number greater than or equal to 10._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" sqref="AP1:AP1048576" xr:uid="{76877D72-6D7B-4053-9D8A-EF5817DEA169}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="LOCUNCM must be a whole number greater than or equal to 10._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" promptTitle="Required field" prompt="Required field" sqref="AP1:AP1048576" xr:uid="{76877D72-6D7B-4053-9D8A-EF5817DEA169}">
       <formula1>10</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="YYYY must have text length = 4._x000a__x000a_See the reference guide at https://github.com/atlanticcanadacdc/template/wiki/Field-metadata#YYYY" sqref="B1:B1048576" xr:uid="{2B2538EA-15F5-4C6F-9BD7-FFFB59409F9B}">
+    <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="YYYY must have text length = 4._x000a__x000a_See the reference guide at https://github.com/atlanticcanadacdc/template/wiki/Field-metadata#YYYY" promptTitle="Required field" prompt="Required field" sqref="B1:B1048576" xr:uid="{2B2538EA-15F5-4C6F-9BD7-FFFB59409F9B}">
       <formula1>4</formula1>
     </dataValidation>
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="ELEVmin must be a whole number greater than or equal to 0._x000a__x000a_See the reference guide at https://github.com/atlanticcanadacdc/template/wiki/Field-metadata#elevmin" sqref="AV1:AV1048576" xr:uid="{9DF3AC12-B532-4B95-9071-2B1B0EC4A8B0}">
@@ -1008,11 +1024,11 @@
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="COLLDUP must be a whole number greater than 0._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" sqref="AK1:AK1048576 AM1:AN1048576 AP1:AP1048576" xr:uid="{C625A903-796B-43AF-B42E-C1CBF9B064D4}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="MM must have a minimum text length of 1 and a maximum text length of 2._x000a__x000a_See the reference guide at https://github.com/atlanticcanadacdc/template/wiki/Field-metadata#mm" sqref="C1:C1048576" xr:uid="{63AA1352-24B0-40CA-9C2F-ED3E31036D5C}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="MM must have a minimum text length of 1 and a maximum text length of 2._x000a__x000a_See the reference guide at https://github.com/atlanticcanadacdc/template/wiki/Field-metadata#mm" promptTitle="Required field" prompt="Required field. If missing use XX" sqref="C1 C3:C1048576 C2" xr:uid="{63AA1352-24B0-40CA-9C2F-ED3E31036D5C}">
       <formula1>1</formula1>
       <formula2>2</formula2>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="DD must have a minimum text length of 1 and a maximum text length of 2._x000a__x000a_See the reference guide at https://github.com/atlanticcanadacdc/template/wiki/Field-metadata#dd" sqref="D1:D1048576" xr:uid="{60512924-9933-4690-BEF6-28C7301C3ABD}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="DD must have a minimum text length of 1 and a maximum text length of 2._x000a__x000a_See the reference guide at https://github.com/atlanticcanadacdc/template/wiki/Field-metadata#dd" promptTitle="Required field" prompt="Required field. If missing use XX" sqref="D1:D2 D4:D1048576 D3" xr:uid="{60512924-9933-4690-BEF6-28C7301C3ABD}">
       <formula1>1</formula1>
       <formula2>2</formula2>
     </dataValidation>
@@ -1020,7 +1036,7 @@
       <formula1>1</formula1>
       <formula2>2</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="LONDEC must have a minimum value of -180 and a maximum value of 180._x000a__x000a_See the reference guide at https://github.com/atlanticcanadacdc/template/wiki/Field-metadata#londec" sqref="AL1:AL4 AL6:AL1048576 AL5" xr:uid="{FBE1E6CF-FE6A-454F-8063-F9B3175370DC}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="LONDEC must have a minimum value of -180 and a maximum value of 180._x000a__x000a_See the reference guide at https://github.com/atlanticcanadacdc/template/wiki/Field-metadata#londec" sqref="AL5 AL6:AL1048576 AL1:AL3 AL4" xr:uid="{FBE1E6CF-FE6A-454F-8063-F9B3175370DC}">
       <formula1>-180</formula1>
       <formula2>180</formula2>
     </dataValidation>
@@ -1055,9 +1071,11 @@
       <formula1>-180</formula1>
       <formula2>180</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Lowercase text only._x000a__x000a_See the reference guide at https://github.com/atlanticcanadacdc/template/wiki/Field-metadata#obevid" sqref="AW1:AW1048576" xr:uid="{F2FE263A-5EDB-45C5-A693-77A7C766B3E0}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Lowercase text only._x000a__x000a_See the reference guide at https://github.com/atlanticcanadacdc/template/wiki/Field-metadata#obevid" promptTitle="Recommended field" prompt="Recommended field" sqref="AW1:AW1048576" xr:uid="{F2FE263A-5EDB-45C5-A693-77A7C766B3E0}">
       <formula1>EXACT(LOWER(AW1),AW1)</formula1>
     </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Required field" prompt="Required field" sqref="N1:N1048576" xr:uid="{D3B06E8A-B02C-42E6-BC1C-28209766C086}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Recommended field" prompt="Recommended field" sqref="AT1:AT1048576" xr:uid="{CB037CEE-1584-4FF3-8A4F-DF7D53480DDD}"/>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" location="refnum" xr:uid="{CB419A17-942D-4C93-A976-F2442794B878}"/>
@@ -1120,9 +1138,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B0B503C-45C2-4682-A279-7D9876A20A9B}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1130,46 +1150,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>55</v>
+      <c r="A2" s="12"/>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>57</v>
+      <c r="A4" s="11" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
+      <c r="A6" s="12" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>54</v>
+      <c r="A7" s="10" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="10"/>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A7" r:id="rId1" display="To make sure you have to most up-to-date version, download the template directly from our repo:" xr:uid="{6915430C-55DD-436F-A74B-E2345D056ECD}"/>
-    <hyperlink ref="A8" r:id="rId2" xr:uid="{DF64407A-3DA9-4C8A-9255-459CE474D232}"/>
-    <hyperlink ref="A5" location="'template_v1-02'!A1" display="template_v1-02" xr:uid="{80375676-F759-4681-9B66-DA4DECEFDFF3}"/>
-    <hyperlink ref="A2" r:id="rId3" xr:uid="{7E898EBA-DAC1-4C2D-A2FF-AE781264A37A}"/>
+    <hyperlink ref="A9" r:id="rId1" display="To make sure you have to most up-to-date version, download the template directly from our repo:" xr:uid="{6915430C-55DD-436F-A74B-E2345D056ECD}"/>
+    <hyperlink ref="A10" r:id="rId2" xr:uid="{DF64407A-3DA9-4C8A-9255-459CE474D232}"/>
+    <hyperlink ref="A7" location="'template_v1-03'!A1" display="template_v1-03" xr:uid="{80375676-F759-4681-9B66-DA4DECEFDFF3}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{7E898EBA-DAC1-4C2D-A2FF-AE781264A37A}"/>
+    <hyperlink ref="A13" r:id="rId4" xr:uid="{6CEE4559-B135-4B11-858D-B54016802669}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
minor tweaks to DET to remove underscore before NOTELOC subfields
remove 1,2,3,4 from internal template
</commit_message>
<xml_diff>
--- a/templates/accdcTemplateOutsideSubmission.xlsx
+++ b/templates/accdcTemplateOutsideSubmission.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pende\Documents\02.1 - WORK AREAS\AC CDC Data Load\template\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{189A1F0A-D370-4D24-9E7F-B1150DCBFD98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{337A04DF-6A3F-49AC-8DF7-3F1EB27D65A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="template_v1-03" sheetId="1" r:id="rId1"/>
+    <sheet name="template_v1-04" sheetId="1" r:id="rId1"/>
     <sheet name="README" sheetId="6" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'template_v1-03'!$A$1:$AZ$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'template_v1-04'!$A$1:$AZ$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -135,18 +135,6 @@
     <t>LONDEC2</t>
   </si>
   <si>
-    <t>_NOTELOCdirections</t>
-  </si>
-  <si>
-    <t>_NOTELOCsurveysite</t>
-  </si>
-  <si>
-    <t>_NOTELOCcoordinates</t>
-  </si>
-  <si>
-    <t>_NOTELOClocuncm</t>
-  </si>
-  <si>
     <t>PROTOCOL</t>
   </si>
   <si>
@@ -202,9 +190,6 @@
   </si>
   <si>
     <t>https://github.com/atlanticcanadacdc/template/wiki</t>
-  </si>
-  <si>
-    <t>template_v1-03</t>
   </si>
   <si>
     <r>
@@ -238,6 +223,21 @@
   </si>
   <si>
     <t>datasubmissions@accdc.ca</t>
+  </si>
+  <si>
+    <t>NOTELOCsurveysite</t>
+  </si>
+  <si>
+    <t>NOTELOCcoordinates</t>
+  </si>
+  <si>
+    <t>NOTELOClocuncm</t>
+  </si>
+  <si>
+    <t>NOTELOCdirections</t>
+  </si>
+  <si>
+    <t>template_v1-04</t>
   </si>
 </sst>
 </file>
@@ -362,7 +362,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -394,9 +394,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -723,7 +720,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AZ2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -782,50 +781,50 @@
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>48</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>52</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="N1" s="14" t="s">
-        <v>45</v>
+      <c r="M1" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="N1" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="O1" s="5" t="s">
         <v>28</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="Q1" s="5" t="s">
         <v>27</v>
@@ -834,7 +833,7 @@
         <v>12</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="T1" s="5" t="s">
         <v>10</v>
@@ -861,22 +860,22 @@
         <v>20</v>
       </c>
       <c r="AB1" s="5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="AC1" s="5" t="s">
         <v>21</v>
       </c>
       <c r="AD1" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="AE1" s="5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="AF1" s="5" t="s">
         <v>22</v>
       </c>
       <c r="AG1" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="AH1" s="5" t="s">
         <v>24</v>
@@ -887,10 +886,10 @@
       <c r="AJ1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AK1" s="14" t="s">
+      <c r="AK1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="AL1" s="14" t="s">
+      <c r="AL1" s="13" t="s">
         <v>7</v>
       </c>
       <c r="AM1" s="5" t="s">
@@ -899,22 +898,22 @@
       <c r="AN1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="AO1" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="AP1" s="14" t="s">
+      <c r="AO1" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="AP1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="AQ1" s="13" t="s">
-        <v>35</v>
+      <c r="AQ1" s="5" t="s">
+        <v>58</v>
       </c>
       <c r="AR1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="AS1" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="AT1" s="14" t="s">
+      <c r="AS1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="AT1" s="13" t="s">
         <v>1</v>
       </c>
       <c r="AU1" s="5" t="s">
@@ -923,17 +922,17 @@
       <c r="AV1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AW1" s="14" t="s">
+      <c r="AW1" s="13" t="s">
         <v>15</v>
       </c>
       <c r="AX1" s="5" t="s">
         <v>23</v>
       </c>
       <c r="AY1" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="AZ1" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:52" s="6" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -1090,7 +1089,7 @@
     <hyperlink ref="J1" r:id="rId10" location="obtimeend" xr:uid="{BFCA50ED-A0E7-4877-B168-34C98CB4A965}"/>
     <hyperlink ref="K1" r:id="rId11" location="subnat" xr:uid="{99199E04-F51F-4470-96BA-FCB038FDF75C}"/>
     <hyperlink ref="L1" r:id="rId12" location="surveysite" xr:uid="{E9AA34AF-10A5-41B1-AC10-9EE443A41E7D}"/>
-    <hyperlink ref="M1" r:id="rId13" location="_notelocsurveysite" xr:uid="{4893B326-A262-46A3-BB78-D31016014B94}"/>
+    <hyperlink ref="M1" r:id="rId13" location="notelocsurveysite" xr:uid="{4893B326-A262-46A3-BB78-D31016014B94}"/>
     <hyperlink ref="N1" r:id="rId14" location="scname" xr:uid="{0A964B0A-5327-4E29-9B5D-921DEE34BB36}"/>
     <hyperlink ref="O1" r:id="rId15" location="nametemp" xr:uid="{4CB1FAE1-9168-4551-9644-D895681F4E7E}"/>
     <hyperlink ref="P1" r:id="rId16" location="common-name" xr:uid="{ACD93D75-78FC-48A8-ACB6-9E2B5A81C6D2}"/>
@@ -1118,18 +1117,18 @@
     <hyperlink ref="AL1" r:id="rId38" location="londec" xr:uid="{834604C0-3879-4AEC-839D-0D78D648EFE3}"/>
     <hyperlink ref="AM1" r:id="rId39" location="latdec2" xr:uid="{83A98BFE-0D53-4943-B7E7-7EF5974C4393}"/>
     <hyperlink ref="AN1" r:id="rId40" location="londec2" xr:uid="{6DB04923-8DE7-4FBD-8A3E-09C02373886A}"/>
-    <hyperlink ref="AO1" r:id="rId41" location="_noteloccoordinates" xr:uid="{98930FB5-28CC-413F-968A-885CA7866F07}"/>
-    <hyperlink ref="AP1" r:id="rId42" location="locuncm" xr:uid="{1525876A-AA09-4E00-9BB8-2442C3E6DB49}"/>
-    <hyperlink ref="AQ1" r:id="rId43" location="_NOTELOClocuncm" xr:uid="{AE3F122D-6433-4CEC-8DE5-E082F33E3E36}"/>
-    <hyperlink ref="AR1" r:id="rId44" location="directions" xr:uid="{A1E53390-1C36-4056-BF37-8BD1B5646CBB}"/>
-    <hyperlink ref="AS1" r:id="rId45" location="_notelocdirections" xr:uid="{67F60461-6A06-4471-AB42-D67B35341E44}"/>
-    <hyperlink ref="AT1" r:id="rId46" location="observer" xr:uid="{F88601D1-DCE8-4E18-A1D1-88E16D02FFDB}"/>
-    <hyperlink ref="AU1" r:id="rId47" location="identby" xr:uid="{D3DE2271-2DE8-448D-B2C1-28E55255E885}"/>
-    <hyperlink ref="AV1" r:id="rId48" location="elevmin" xr:uid="{8F13C8E8-B3AA-425C-AF41-E52081E81C65}"/>
-    <hyperlink ref="AW1" r:id="rId49" location="obevid" xr:uid="{3571114C-8AC4-44B0-ADC7-F28FE53ECA68}"/>
-    <hyperlink ref="AX1" r:id="rId50" location="collection" xr:uid="{93D60417-BCDE-4324-B0FD-34842EC37569}"/>
-    <hyperlink ref="AY1" r:id="rId51" location="note1" xr:uid="{AF0D8176-10CC-4474-8491-EE0D335AAFC0}"/>
-    <hyperlink ref="AZ1" r:id="rId52" location="note2" xr:uid="{4668AA28-2B31-4422-8FAF-A3AFFC4FC986}"/>
+    <hyperlink ref="AP1" r:id="rId41" location="locuncm" xr:uid="{1525876A-AA09-4E00-9BB8-2442C3E6DB49}"/>
+    <hyperlink ref="AQ1" r:id="rId42" location="NOTELOClocuncm" xr:uid="{AE3F122D-6433-4CEC-8DE5-E082F33E3E36}"/>
+    <hyperlink ref="AR1" r:id="rId43" location="directions" xr:uid="{A1E53390-1C36-4056-BF37-8BD1B5646CBB}"/>
+    <hyperlink ref="AS1" r:id="rId44" location="notelocdirections" xr:uid="{67F60461-6A06-4471-AB42-D67B35341E44}"/>
+    <hyperlink ref="AT1" r:id="rId45" location="observer" xr:uid="{F88601D1-DCE8-4E18-A1D1-88E16D02FFDB}"/>
+    <hyperlink ref="AU1" r:id="rId46" location="identby" xr:uid="{D3DE2271-2DE8-448D-B2C1-28E55255E885}"/>
+    <hyperlink ref="AV1" r:id="rId47" location="elevmin" xr:uid="{8F13C8E8-B3AA-425C-AF41-E52081E81C65}"/>
+    <hyperlink ref="AW1" r:id="rId48" location="obevid" xr:uid="{3571114C-8AC4-44B0-ADC7-F28FE53ECA68}"/>
+    <hyperlink ref="AX1" r:id="rId49" location="collection" xr:uid="{93D60417-BCDE-4324-B0FD-34842EC37569}"/>
+    <hyperlink ref="AY1" r:id="rId50" location="note1" xr:uid="{AF0D8176-10CC-4474-8491-EE0D335AAFC0}"/>
+    <hyperlink ref="AZ1" r:id="rId51" location="note2" xr:uid="{4668AA28-2B31-4422-8FAF-A3AFFC4FC986}"/>
+    <hyperlink ref="AO1" r:id="rId52" location="noteloccoordinates" xr:uid="{98930FB5-28CC-413F-968A-885CA7866F07}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId53"/>
@@ -1151,7 +1150,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -1159,22 +1158,22 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
@@ -1182,29 +1181,29 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A9" r:id="rId1" display="To make sure you have to most up-to-date version, download the template directly from our repo:" xr:uid="{6915430C-55DD-436F-A74B-E2345D056ECD}"/>
     <hyperlink ref="A10" r:id="rId2" xr:uid="{DF64407A-3DA9-4C8A-9255-459CE474D232}"/>
-    <hyperlink ref="A7" location="'template_v1-03'!A1" display="template_v1-03" xr:uid="{80375676-F759-4681-9B66-DA4DECEFDFF3}"/>
+    <hyperlink ref="A7" location="'template_v1-04'!A1" display="template_v1-04" xr:uid="{80375676-F759-4681-9B66-DA4DECEFDFF3}"/>
     <hyperlink ref="A4" r:id="rId3" xr:uid="{7E898EBA-DAC1-4C2D-A2FF-AE781264A37A}"/>
     <hyperlink ref="A13" r:id="rId4" xr:uid="{6CEE4559-B135-4B11-858D-B54016802669}"/>
   </hyperlinks>

</xml_diff>